<commit_message>
code fix after zoom with Rami 6/6 without fix evaluation
</commit_message>
<xml_diff>
--- a/Semester_B/תוצאות ניסויים.xlsx
+++ b/Semester_B/תוצאות ניסויים.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayz\OneDrive - post.bgu.ac.il\שולחן העבודה\Study\שנה ה 2023 - 2024\סמסטר א\פרויקט מסכם 1\פרויקט\08 ProjectCode\Semester_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2626D1D-E70E-448B-B51C-6C24A5ED0841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC44F37-064B-440B-BFCD-110DF3F28412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
     </r>
   </si>
   <si>
-    <t>FIX prompt (limit return to 3 rules only)</t>
+    <t>FIX prompt (limit return to 2 rules only)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,6 +577,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -660,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -689,6 +695,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -705,6 +720,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -990,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,24 +1030,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:17" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="H2" s="10" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="H2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
-      <c r="N2" s="10" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+      <c r="N2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="12"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="15"/>
     </row>
     <row r="3" spans="1:17" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -1250,7 +1274,7 @@
       <c r="C10" s="2">
         <v>0.08</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>0.3</v>
       </c>
       <c r="E10" s="2">
@@ -1273,114 +1297,114 @@
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="10">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
       <c r="N11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="10">
         <v>0.08</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="11">
         <v>0.12</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
       <c r="N12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="1"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="11"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
     </row>
     <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="H20" s="10" t="s">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="H20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="N20" s="10" t="s">
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="17"/>
+      <c r="N20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="12"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
@@ -1424,9 +1448,15 @@
       <c r="B22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="9"/>
+      <c r="C22" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.18</v>
+      </c>
       <c r="H22" s="7" t="s">
         <v>9</v>
       </c>
@@ -1450,9 +1480,15 @@
       <c r="B23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="9"/>
+      <c r="C23" s="8">
+        <v>0.23</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="E23" s="20">
+        <v>0.21</v>
+      </c>
       <c r="H23" s="7" t="s">
         <v>10</v>
       </c>
@@ -1508,9 +1544,15 @@
       <c r="B25" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="C25" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.11</v>
+      </c>
       <c r="H25" s="7" t="s">
         <v>8</v>
       </c>
@@ -1528,9 +1570,15 @@
       <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="C26" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.17</v>
+      </c>
       <c r="H26" s="7" t="s">
         <v>11</v>
       </c>
@@ -1548,9 +1596,15 @@
       <c r="B27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="C27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.12</v>
+      </c>
       <c r="H27" s="7" t="s">
         <v>12</v>
       </c>
@@ -1568,9 +1622,15 @@
       <c r="B28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H28" s="7" t="s">
         <v>13</v>
       </c>
@@ -1588,9 +1648,15 @@
       <c r="B29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="C29" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.13</v>
+      </c>
       <c r="H29" s="7" t="s">
         <v>15</v>
       </c>
@@ -1608,9 +1674,15 @@
       <c r="B30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="1"/>
+      <c r="C30" s="19">
+        <v>0.22</v>
+      </c>
+      <c r="D30" s="19">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0.23</v>
+      </c>
       <c r="H30" s="7" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Finish run exp (Claude)
</commit_message>
<xml_diff>
--- a/Semester_B/תוצאות ניסויים.xlsx
+++ b/Semester_B/תוצאות ניסויים.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shayz\OneDrive - post.bgu.ac.il\שולחן העבודה\Study\שנה ה 2023 - 2024\סמסטר א\פרויקט מסכם 1\פרויקט\08 ProjectCode\Semester_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246CB20F-6F3A-4483-A1E8-0B13487EABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B21FE72-EFFD-49AB-9635-E6C2FD11492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Gemini" sheetId="2" r:id="rId2"/>
+    <sheet name="GPT" sheetId="3" r:id="rId3"/>
+    <sheet name="CLAUDE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1555,7 +1557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1677,9 +1679,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1783,6 +1782,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1810,10 +1812,7 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1840,6 +1839,753 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95522</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>13064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>168728</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>96884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB78738-7534-3D0D-1010-D09B94179B3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7878808" y="516528"/>
+          <a:ext cx="12931956" cy="5614307"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EE06044-D39B-907A-660C-E2E9B7E99B14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7764780" y="6537960"/>
+          <a:ext cx="13152120" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5E06025-78C1-588D-DC68-BF7731E3777D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7764780" y="12573000"/>
+          <a:ext cx="13152120" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>340179</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>137432</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>160564</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D75BAD9E-561D-E064-BB83-ED9458058A9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7511143" y="18832285"/>
+          <a:ext cx="13268325" cy="5440136"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB5E5E79-A52D-5046-C71A-8DBAC83DC4D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13243560" cy="5608320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FC1FEFC-8327-16FF-C883-D9C2E7B6ED6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6035040"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BAA2486-237B-472A-296C-117CA41CFD89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="12070080"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F07CEA54-3E66-4B28-2568-6797055778E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="18105120"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82AB2B02-0A50-A289-06F3-329D9DC0F0B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13228320" cy="5608320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8201E3C3-C854-CDFB-AA01-6A61ED8A2B30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="6035040"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55433E11-914E-5F19-21B7-BA6B99EA4ED2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="12252960"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F33AEB-7E78-0DCB-C3E4-0063B6957EEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="18288000"/>
+          <a:ext cx="13144500" cy="5623560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2107,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2500,16 +3246,16 @@
       <c r="Q20" s="82"/>
     </row>
     <row r="21" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="45" t="s">
         <v>1</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -2538,19 +3284,19 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="51">
+      <c r="C22" s="50">
         <v>0.16</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="50">
         <v>0.2</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="51">
         <v>0.18</v>
       </c>
-      <c r="H22" s="65" t="s">
+      <c r="H22" s="64" t="s">
         <v>55</v>
       </c>
       <c r="I22" s="2">
@@ -2562,7 +3308,7 @@
       <c r="K22" s="1">
         <v>0.3</v>
       </c>
-      <c r="N22" s="65" t="s">
+      <c r="N22" s="64" t="s">
         <v>55</v>
       </c>
       <c r="O22" s="8">
@@ -2576,19 +3322,19 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="53">
+      <c r="C23" s="52">
         <v>0.23</v>
       </c>
-      <c r="D23" s="53">
+      <c r="D23" s="52">
         <v>0.32</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="53">
         <v>0.21</v>
       </c>
-      <c r="H23" s="63" t="s">
+      <c r="H23" s="62" t="s">
         <v>56</v>
       </c>
       <c r="I23" s="8">
@@ -2600,7 +3346,7 @@
       <c r="K23" s="9">
         <v>0.45</v>
       </c>
-      <c r="N23" s="63" t="s">
+      <c r="N23" s="62" t="s">
         <v>56</v>
       </c>
       <c r="O23" s="2">
@@ -2652,19 +3398,19 @@
       </c>
     </row>
     <row r="25" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="55">
+      <c r="C25" s="54">
         <v>0.1</v>
       </c>
-      <c r="D25" s="55">
+      <c r="D25" s="54">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E25" s="56">
+      <c r="E25" s="55">
         <v>0.11</v>
       </c>
-      <c r="H25" s="62" t="s">
+      <c r="H25" s="61" t="s">
         <v>51</v>
       </c>
       <c r="I25" s="10">
@@ -2676,7 +3422,7 @@
       <c r="K25" s="11">
         <v>0.19</v>
       </c>
-      <c r="N25" s="62" t="s">
+      <c r="N25" s="61" t="s">
         <v>51</v>
       </c>
       <c r="O25" s="10"/>
@@ -2684,19 +3430,19 @@
       <c r="Q25" s="10"/>
     </row>
     <row r="26" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="58" t="s">
+      <c r="B26" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="41">
         <v>0.18</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="41">
         <v>0.22</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="41">
         <v>0.2</v>
       </c>
-      <c r="H26" s="58" t="s">
+      <c r="H26" s="57" t="s">
         <v>57</v>
       </c>
       <c r="I26" s="2">
@@ -2708,7 +3454,7 @@
       <c r="K26" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="N26" s="58" t="s">
+      <c r="N26" s="57" t="s">
         <v>57</v>
       </c>
       <c r="O26" s="2"/>
@@ -2719,13 +3465,13 @@
       <c r="B27" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="41">
         <v>0.18</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="41">
         <v>0.22</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="41">
         <v>0.2</v>
       </c>
       <c r="H27" s="21" t="s">
@@ -2742,25 +3488,25 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="47">
         <v>0.1</v>
       </c>
-      <c r="D28" s="55">
+      <c r="D28" s="54">
         <v>0.15</v>
       </c>
-      <c r="E28" s="48">
+      <c r="E28" s="47">
         <v>0.12</v>
       </c>
-      <c r="H28" s="62" t="s">
+      <c r="H28" s="61" t="s">
         <v>52</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
-      <c r="N28" s="62" t="s">
+      <c r="N28" s="61" t="s">
         <v>52</v>
       </c>
       <c r="O28" s="10"/>
@@ -2768,25 +3514,25 @@
       <c r="Q28" s="10"/>
     </row>
     <row r="29" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="47">
+      <c r="C29" s="46">
         <v>0.16</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="41">
         <v>0.22</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="46">
         <v>0.18</v>
       </c>
-      <c r="H29" s="59" t="s">
+      <c r="H29" s="58" t="s">
         <v>58</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="N29" s="59" t="s">
+      <c r="N29" s="58" t="s">
         <v>58</v>
       </c>
       <c r="O29" s="2"/>
@@ -2820,25 +3566,25 @@
       <c r="Q30" s="2"/>
     </row>
     <row r="31" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="57">
+      <c r="C31" s="56">
         <v>0.12</v>
       </c>
-      <c r="D31" s="57">
+      <c r="D31" s="56">
         <v>0.15</v>
       </c>
-      <c r="E31" s="57">
+      <c r="E31" s="56">
         <v>0.13</v>
       </c>
-      <c r="H31" s="64" t="s">
+      <c r="H31" s="63" t="s">
         <v>60</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-      <c r="N31" s="64" t="s">
+      <c r="N31" s="63" t="s">
         <v>60</v>
       </c>
       <c r="O31" s="2"/>
@@ -2872,68 +3618,68 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="48">
         <v>0.16</v>
       </c>
-      <c r="D33" s="49">
+      <c r="D33" s="48">
         <v>0.19</v>
       </c>
-      <c r="E33" s="50">
+      <c r="E33" s="49">
         <v>0.18</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="I33" s="61"/>
+      <c r="I33" s="60"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1"/>
       <c r="N33" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="O33" s="61"/>
+      <c r="O33" s="60"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="1"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="76"/>
-      <c r="F36" s="76"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="76"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="76"/>
-      <c r="Q36" s="76"/>
+      <c r="A36" s="75"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="75"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="75"/>
+      <c r="L36" s="75"/>
+      <c r="M36" s="75"/>
+      <c r="N36" s="75"/>
+      <c r="O36" s="75"/>
+      <c r="P36" s="75"/>
+      <c r="Q36" s="75"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="76"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="76"/>
-      <c r="Q37" s="76"/>
+      <c r="A37" s="75"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
+      <c r="O37" s="75"/>
+      <c r="P37" s="75"/>
+      <c r="Q37" s="75"/>
     </row>
     <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2957,57 +3703,57 @@
       <c r="Q40" s="79"/>
     </row>
     <row r="41" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="72" t="s">
+      <c r="C41" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="73" t="s">
+      <c r="D41" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="74" t="s">
+      <c r="E41" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="71" t="s">
+      <c r="H41" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I41" s="72" t="s">
+      <c r="I41" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="J41" s="73" t="s">
+      <c r="J41" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="K41" s="74" t="s">
+      <c r="K41" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="N41" s="71" t="s">
+      <c r="N41" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="O41" s="72" t="s">
+      <c r="O41" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="P41" s="73" t="s">
+      <c r="P41" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="Q41" s="74" t="s">
+      <c r="Q41" s="73" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="51">
+      <c r="C42" s="50">
         <v>0.16</v>
       </c>
-      <c r="D42" s="51">
+      <c r="D42" s="50">
         <v>0.2</v>
       </c>
-      <c r="E42" s="52">
+      <c r="E42" s="51">
         <v>0.18</v>
       </c>
-      <c r="H42" s="66" t="s">
+      <c r="H42" s="65" t="s">
         <v>55</v>
       </c>
       <c r="I42" s="2">
@@ -3019,7 +3765,7 @@
       <c r="K42" s="1">
         <v>0.3</v>
       </c>
-      <c r="N42" s="66" t="s">
+      <c r="N42" s="65" t="s">
         <v>55</v>
       </c>
       <c r="O42" s="8">
@@ -3036,22 +3782,22 @@
       <c r="A43" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="53">
+      <c r="C43" s="52">
         <v>0.23</v>
       </c>
-      <c r="D43" s="53">
+      <c r="D43" s="52">
         <v>0.32</v>
       </c>
-      <c r="E43" s="54">
+      <c r="E43" s="53">
         <v>0.21</v>
       </c>
       <c r="G43" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="66" t="s">
+      <c r="H43" s="65" t="s">
         <v>56</v>
       </c>
       <c r="I43" s="8">
@@ -3063,7 +3809,7 @@
       <c r="K43" s="9">
         <v>0.45</v>
       </c>
-      <c r="N43" s="66" t="s">
+      <c r="N43" s="65" t="s">
         <v>56</v>
       </c>
       <c r="O43" s="2">
@@ -3077,18 +3823,18 @@
       </c>
     </row>
     <row r="44" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="67"/>
-      <c r="C44" s="68"/>
-      <c r="D44" s="68"/>
-      <c r="E44" s="69"/>
-      <c r="H44" s="67"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="68"/>
-      <c r="K44" s="69"/>
-      <c r="N44" s="67"/>
-      <c r="O44" s="68"/>
-      <c r="P44" s="68"/>
-      <c r="Q44" s="69"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="68"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="68"/>
+      <c r="N44" s="66"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="67"/>
+      <c r="Q44" s="68"/>
     </row>
     <row r="45" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="40" t="s">
@@ -3129,92 +3875,98 @@
       </c>
     </row>
     <row r="46" spans="1:17" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="57">
+      <c r="C46" s="56">
         <v>0.12</v>
       </c>
-      <c r="D46" s="57">
+      <c r="D46" s="56">
         <v>0.15</v>
       </c>
-      <c r="E46" s="57">
+      <c r="E46" s="56">
         <v>0.13</v>
       </c>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="I46" s="57">
+      <c r="I46" s="56">
         <v>0.16</v>
       </c>
-      <c r="J46" s="57">
+      <c r="J46" s="56">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K46" s="57">
+      <c r="K46" s="56">
         <v>0.2</v>
       </c>
-      <c r="N46" s="64" t="s">
+      <c r="N46" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="O46" s="57">
+      <c r="O46" s="56">
         <v>0.19</v>
       </c>
-      <c r="P46" s="57">
+      <c r="P46" s="56">
         <v>0.21</v>
       </c>
-      <c r="Q46" s="57">
+      <c r="Q46" s="56">
         <v>0.2</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="70"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="56"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="56"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="55"/>
-      <c r="P47" s="55"/>
-      <c r="Q47" s="56"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="55"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="55"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="54"/>
+      <c r="P47" s="54"/>
+      <c r="Q47" s="55"/>
     </row>
     <row r="48" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="42">
+      <c r="C48" s="41">
         <v>0.18</v>
       </c>
-      <c r="D48" s="42">
+      <c r="D48" s="41">
         <v>0.22</v>
       </c>
-      <c r="E48" s="42">
+      <c r="E48" s="41">
         <v>0.2</v>
       </c>
       <c r="G48" t="s">
         <v>61</v>
       </c>
-      <c r="H48" s="58" t="s">
+      <c r="H48" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="I48" s="86"/>
-      <c r="J48" s="86"/>
-      <c r="K48" s="86"/>
-      <c r="N48" s="58" t="s">
+      <c r="I48" s="6">
+        <v>0.21</v>
+      </c>
+      <c r="J48" s="41">
+        <v>0.39</v>
+      </c>
+      <c r="K48" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="N48" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="O48" s="86">
+      <c r="O48" s="6">
         <v>0.23</v>
       </c>
-      <c r="P48" s="86">
+      <c r="P48" s="6">
         <v>0.3</v>
       </c>
-      <c r="Q48" s="86">
+      <c r="Q48" s="6">
         <v>0.26</v>
       </c>
     </row>
@@ -3225,13 +3977,13 @@
       <c r="B49" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="42">
+      <c r="C49" s="41">
         <v>0.18</v>
       </c>
-      <c r="D49" s="42">
+      <c r="D49" s="41">
         <v>0.22</v>
       </c>
-      <c r="E49" s="42">
+      <c r="E49" s="41">
         <v>0.2</v>
       </c>
       <c r="G49" t="s">
@@ -3240,19 +3992,25 @@
       <c r="H49" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I49" s="86"/>
-      <c r="J49" s="86"/>
-      <c r="K49" s="86"/>
+      <c r="I49" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="J49" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="K49" s="6">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="N49" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="O49" s="86">
+      <c r="O49" s="6">
         <v>0.23</v>
       </c>
-      <c r="P49" s="86">
+      <c r="P49" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="Q49" s="86">
+      <c r="Q49" s="6">
         <v>0.26</v>
       </c>
     </row>
@@ -3260,34 +4018,40 @@
       <c r="A50" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="59" t="s">
+      <c r="B50" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="47">
+      <c r="C50" s="46">
         <v>0.16</v>
       </c>
-      <c r="D50" s="42">
+      <c r="D50" s="41">
         <v>0.22</v>
       </c>
-      <c r="E50" s="47">
+      <c r="E50" s="46">
         <v>0.18</v>
       </c>
-      <c r="H50" s="59" t="s">
+      <c r="H50" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="I50" s="75"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="75"/>
-      <c r="N50" s="59" t="s">
+      <c r="I50" s="76">
+        <v>0.25</v>
+      </c>
+      <c r="J50" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="K50" s="74">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N50" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="O50" s="87">
+      <c r="O50" s="76">
         <v>0.28000000000000003</v>
       </c>
-      <c r="P50" s="42">
+      <c r="P50" s="41">
         <v>0.33</v>
       </c>
-      <c r="Q50" s="87">
+      <c r="Q50" s="76">
         <v>0.31</v>
       </c>
     </row>
@@ -3310,13 +4074,19 @@
       <c r="H51" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="I51" s="76">
+        <v>0.25</v>
+      </c>
+      <c r="J51" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="K51" s="76">
+        <v>0.3</v>
+      </c>
       <c r="N51" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="O51" s="42">
+      <c r="O51" s="41">
         <v>0.28000000000000003</v>
       </c>
       <c r="P51" s="2">
@@ -3342,9 +4112,15 @@
       <c r="H52" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="39"/>
+      <c r="I52" s="86">
+        <v>0.25</v>
+      </c>
+      <c r="J52" s="13">
+        <v>0.36</v>
+      </c>
+      <c r="K52" s="39">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="N52" s="29" t="s">
         <v>59</v>
       </c>
@@ -3359,31 +4135,37 @@
       </c>
     </row>
     <row r="53" spans="1:17" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="60" t="s">
+      <c r="B53" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="49">
+      <c r="C53" s="48">
         <v>0.16</v>
       </c>
-      <c r="D53" s="49">
+      <c r="D53" s="48">
         <v>0.21</v>
       </c>
-      <c r="E53" s="50">
+      <c r="E53" s="49">
         <v>0.18</v>
       </c>
-      <c r="H53" s="60" t="s">
+      <c r="H53" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49"/>
-      <c r="K53" s="50"/>
-      <c r="N53" s="60" t="s">
+      <c r="I53" s="86">
+        <v>0.25</v>
+      </c>
+      <c r="J53" s="13">
+        <v>0.36</v>
+      </c>
+      <c r="K53" s="39">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N53" s="59" t="s">
         <v>54</v>
       </c>
       <c r="O53" s="13">
         <v>0.26</v>
       </c>
-      <c r="P53" s="49">
+      <c r="P53" s="48">
         <v>0.28999999999999998</v>
       </c>
       <c r="Q53" s="39">
@@ -3412,8 +4194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D97262-586D-4AA2-A676-C5BE1616E623}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3952,5 +4734,36 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F40B65F-8508-4210-8B40-72E1C37E06F1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="Y61" sqref="Y61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B42BB4D-E5AF-4045-92FF-C7D076200934}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="Y103" sqref="Y103"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>